<commit_message>
Updated fees xlss, and found bug in updatevaultsIssuances where there was == instead of =
</commit_message>
<xml_diff>
--- a/results/FeeAnalysis.xlsx
+++ b/results/FeeAnalysis.xlsx
@@ -88,7 +88,7 @@
     <t xml:space="preserve">2^l/[1+(l-1)fBase]^2</t>
   </si>
   <si>
-    <t xml:space="preserve">[1+(l-1)fBase]-1</t>
+    <t xml:space="preserve">1/[1+(l-1)fBase]-1</t>
   </si>
   <si>
     <t xml:space="preserve">[1+(l-1)fBase]^(-2)-1</t>
@@ -108,6 +108,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -129,6 +130,7 @@
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -141,6 +143,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -209,68 +212,72 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -354,7 +361,7 @@
   <dimension ref="B1:L18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.48828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -440,47 +447,47 @@
       <c r="J10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K10" s="0"/>
-      <c r="L10" s="0"/>
-    </row>
-    <row r="11" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="10" t="s">
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+    </row>
+    <row r="11" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="J11" s="9" t="s">
+      <c r="J11" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="12" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="11" t="n">
+      <c r="B12" s="12" t="n">
         <v>-4</v>
       </c>
       <c r="C12" s="2" t="n">
         <f aca="false">1+2^B12</f>
         <v>1.0625</v>
       </c>
-      <c r="D12" s="11" t="str">
+      <c r="D12" s="12" t="str">
         <f aca="false">ROUND(100*((1+(C12-1)*C$3)^(2/(C12-1))-1),0) &amp; "%"</f>
         <v>120%</v>
       </c>
@@ -500,24 +507,24 @@
         <f aca="false">ROUND(100*(2^C12/(1+(C12-1)*C$3)^2-1),0) &amp; "%"</f>
         <v>99%</v>
       </c>
-      <c r="I12" s="12" t="str">
+      <c r="I12" s="13" t="str">
         <f aca="false">ROUND(100*(1/(1+(C12-1)*C$3)-1),0) &amp; "%"</f>
         <v>-2%</v>
       </c>
-      <c r="J12" s="12" t="str">
+      <c r="J12" s="13" t="str">
         <f aca="false">ROUND(100*((1+(C12-1)*C$3)^(-2)-1),0) &amp; "%"</f>
         <v>-5%</v>
       </c>
     </row>
     <row r="13" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="11" t="n">
+      <c r="B13" s="12" t="n">
         <v>-3</v>
       </c>
       <c r="C13" s="2" t="n">
         <f aca="false">1+2^B13</f>
         <v>1.125</v>
       </c>
-      <c r="D13" s="11" t="str">
+      <c r="D13" s="12" t="str">
         <f aca="false">ROUND(100*((1+(C13-1)*C$3)^(2/(C13-1))-1),0) &amp; "%"</f>
         <v>118%</v>
       </c>
@@ -537,24 +544,24 @@
         <f aca="false">ROUND(100*(2^C13/(1+(C13-1)*C$3)^2-1),0) &amp; "%"</f>
         <v>98%</v>
       </c>
-      <c r="I13" s="12" t="str">
+      <c r="I13" s="13" t="str">
         <f aca="false">ROUND(100*(1/(1+(C13-1)*C$3)-1),0) &amp; "%"</f>
         <v>-5%</v>
       </c>
-      <c r="J13" s="12" t="str">
+      <c r="J13" s="13" t="str">
         <f aca="false">ROUND(100*((1+(C13-1)*C$3)^(-2)-1),0) &amp; "%"</f>
         <v>-9%</v>
       </c>
     </row>
     <row r="14" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="11" t="n">
+      <c r="B14" s="12" t="n">
         <v>-2</v>
       </c>
       <c r="C14" s="2" t="n">
         <f aca="false">1+2^B14</f>
         <v>1.25</v>
       </c>
-      <c r="D14" s="11" t="str">
+      <c r="D14" s="12" t="str">
         <f aca="false">ROUND(100*((1+(C14-1)*C$3)^(2/(C14-1))-1),0) &amp; "%"</f>
         <v>114%</v>
       </c>
@@ -574,61 +581,61 @@
         <f aca="false">ROUND(100*(2^C14/(1+(C14-1)*C$3)^2-1),0) &amp; "%"</f>
         <v>97%</v>
       </c>
-      <c r="I14" s="12" t="str">
+      <c r="I14" s="13" t="str">
         <f aca="false">ROUND(100*(1/(1+(C14-1)*C$3)-1),0) &amp; "%"</f>
         <v>-9%</v>
       </c>
-      <c r="J14" s="12" t="str">
+      <c r="J14" s="13" t="str">
         <f aca="false">ROUND(100*((1+(C14-1)*C$3)^(-2)-1),0) &amp; "%"</f>
         <v>-17%</v>
       </c>
     </row>
     <row r="15" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="13" t="n">
+      <c r="B15" s="14" t="n">
         <v>-1</v>
       </c>
-      <c r="C15" s="14" t="n">
+      <c r="C15" s="15" t="n">
         <f aca="false">1+2^B15</f>
         <v>1.5</v>
       </c>
-      <c r="D15" s="13" t="str">
+      <c r="D15" s="14" t="str">
         <f aca="false">ROUND(100*((1+(C15-1)*C$3)^(2/(C15-1))-1),0) &amp; "%"</f>
         <v>107%</v>
       </c>
-      <c r="E15" s="14" t="str">
+      <c r="E15" s="15" t="str">
         <f aca="false">ROUND(100*((1+(C15-1)*C$3)^(2/C15)-1),0) &amp; "%"</f>
         <v>28%</v>
       </c>
-      <c r="F15" s="14" t="str">
+      <c r="F15" s="15" t="str">
         <f aca="false">ROUND(100*(2^(C15-1)/(1+(C15-1)*C$3)^2-1),0) &amp; "%"</f>
         <v>-2%</v>
       </c>
-      <c r="G15" s="14" t="str">
+      <c r="G15" s="15" t="str">
         <f aca="false">ROUND(100*(10^(C15-1)/(1+(C15-1)*C$3)^2-1),0) &amp; "%"</f>
         <v>120%</v>
       </c>
-      <c r="H15" s="14" t="str">
+      <c r="H15" s="15" t="str">
         <f aca="false">ROUND(100*(2^C15/(1+(C15-1)*C$3)^2-1),0) &amp; "%"</f>
         <v>96%</v>
       </c>
-      <c r="I15" s="15" t="str">
+      <c r="I15" s="16" t="str">
         <f aca="false">ROUND(100*(1/(1+(C15-1)*C$3)-1),0) &amp; "%"</f>
         <v>-17%</v>
       </c>
-      <c r="J15" s="15" t="str">
+      <c r="J15" s="16" t="str">
         <f aca="false">ROUND(100*((1+(C15-1)*C$3)^(-2)-1),0) &amp; "%"</f>
         <v>-31%</v>
       </c>
     </row>
     <row r="16" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="11" t="n">
+      <c r="B16" s="12" t="n">
         <v>0</v>
       </c>
       <c r="C16" s="2" t="n">
         <f aca="false">1+2^B16</f>
         <v>2</v>
       </c>
-      <c r="D16" s="11" t="str">
+      <c r="D16" s="12" t="str">
         <f aca="false">ROUND(100*((1+(C16-1)*C$3)^(2/(C16-1))-1),0) &amp; "%"</f>
         <v>96%</v>
       </c>
@@ -648,24 +655,24 @@
         <f aca="false">ROUND(100*(2^C16/(1+(C16-1)*C$3)^2-1),0) &amp; "%"</f>
         <v>104%</v>
       </c>
-      <c r="I16" s="12" t="str">
+      <c r="I16" s="13" t="str">
         <f aca="false">ROUND(100*(1/(1+(C16-1)*C$3)-1),0) &amp; "%"</f>
         <v>-29%</v>
       </c>
-      <c r="J16" s="12" t="str">
+      <c r="J16" s="13" t="str">
         <f aca="false">ROUND(100*((1+(C16-1)*C$3)^(-2)-1),0) &amp; "%"</f>
         <v>-49%</v>
       </c>
     </row>
     <row r="17" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="11" t="n">
+      <c r="B17" s="12" t="n">
         <v>1</v>
       </c>
       <c r="C17" s="2" t="n">
         <f aca="false">1+2^B17</f>
         <v>3</v>
       </c>
-      <c r="D17" s="11" t="str">
+      <c r="D17" s="12" t="str">
         <f aca="false">ROUND(100*((1+(C17-1)*C$3)^(2/(C17-1))-1),0) &amp; "%"</f>
         <v>80%</v>
       </c>
@@ -685,24 +692,24 @@
         <f aca="false">ROUND(100*(2^C17/(1+(C17-1)*C$3)^2-1),0) &amp; "%"</f>
         <v>147%</v>
       </c>
-      <c r="I17" s="12" t="str">
+      <c r="I17" s="13" t="str">
         <f aca="false">ROUND(100*(1/(1+(C17-1)*C$3)-1),0) &amp; "%"</f>
         <v>-44%</v>
       </c>
-      <c r="J17" s="12" t="str">
+      <c r="J17" s="13" t="str">
         <f aca="false">ROUND(100*((1+(C17-1)*C$3)^(-2)-1),0) &amp; "%"</f>
         <v>-69%</v>
       </c>
     </row>
     <row r="18" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="11" t="n">
+      <c r="B18" s="12" t="n">
         <v>2</v>
       </c>
       <c r="C18" s="2" t="n">
         <f aca="false">1+2^B18</f>
         <v>5</v>
       </c>
-      <c r="D18" s="11" t="str">
+      <c r="D18" s="12" t="str">
         <f aca="false">ROUND(100*((1+(C18-1)*C$3)^(2/(C18-1))-1),0) &amp; "%"</f>
         <v>61%</v>
       </c>
@@ -722,11 +729,11 @@
         <f aca="false">ROUND(100*(2^C18/(1+(C18-1)*C$3)^2-1),0) &amp; "%"</f>
         <v>373%</v>
       </c>
-      <c r="I18" s="12" t="str">
+      <c r="I18" s="13" t="str">
         <f aca="false">ROUND(100*(1/(1+(C18-1)*C$3)-1),0) &amp; "%"</f>
         <v>-62%</v>
       </c>
-      <c r="J18" s="12" t="str">
+      <c r="J18" s="13" t="str">
         <f aca="false">ROUND(100*((1+(C18-1)*C$3)^(-2)-1),0) &amp; "%"</f>
         <v>-85%</v>
       </c>

</xml_diff>

<commit_message>
further fee simplifications, POL also receives its fair share of fees from the apes
</commit_message>
<xml_diff>
--- a/results/FeeAnalysis.xlsx
+++ b/results/FeeAnalysis.xlsx
@@ -361,7 +361,7 @@
   <dimension ref="B1:L18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.48828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -381,7 +381,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -489,23 +489,23 @@
       </c>
       <c r="D12" s="12" t="str">
         <f aca="false">ROUND(100*((1+(C12-1)*C$3)^(2/(C12-1))-1),0) &amp; "%"</f>
-        <v>120%</v>
+        <v>81%</v>
       </c>
       <c r="E12" s="2" t="str">
         <f aca="false">ROUND(100*((1+(C12-1)*C$3)^(2/C12)-1),0) &amp; "%"</f>
-        <v>5%</v>
+        <v>4%</v>
       </c>
       <c r="F12" s="2" t="str">
         <f aca="false">ROUND(100*(2^(C12-1)/(1+(C12-1)*C$3)^2-1),0) &amp; "%"</f>
-        <v>-1%</v>
+        <v>1%</v>
       </c>
       <c r="G12" s="2" t="str">
         <f aca="false">ROUND(100*(10^(C12-1)/(1+(C12-1)*C$3)^2-1),0) &amp; "%"</f>
-        <v>10%</v>
+        <v>11%</v>
       </c>
       <c r="H12" s="2" t="str">
         <f aca="false">ROUND(100*(2^C12/(1+(C12-1)*C$3)^2-1),0) &amp; "%"</f>
-        <v>99%</v>
+        <v>101%</v>
       </c>
       <c r="I12" s="13" t="str">
         <f aca="false">ROUND(100*(1/(1+(C12-1)*C$3)-1),0) &amp; "%"</f>
@@ -513,7 +513,7 @@
       </c>
       <c r="J12" s="13" t="str">
         <f aca="false">ROUND(100*((1+(C12-1)*C$3)^(-2)-1),0) &amp; "%"</f>
-        <v>-5%</v>
+        <v>-4%</v>
       </c>
     </row>
     <row r="13" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -526,31 +526,31 @@
       </c>
       <c r="D13" s="12" t="str">
         <f aca="false">ROUND(100*((1+(C13-1)*C$3)^(2/(C13-1))-1),0) &amp; "%"</f>
-        <v>118%</v>
+        <v>80%</v>
       </c>
       <c r="E13" s="2" t="str">
         <f aca="false">ROUND(100*((1+(C13-1)*C$3)^(2/C13)-1),0) &amp; "%"</f>
-        <v>9%</v>
+        <v>7%</v>
       </c>
       <c r="F13" s="2" t="str">
         <f aca="false">ROUND(100*(2^(C13-1)/(1+(C13-1)*C$3)^2-1),0) &amp; "%"</f>
-        <v>-1%</v>
+        <v>1%</v>
       </c>
       <c r="G13" s="2" t="str">
         <f aca="false">ROUND(100*(10^(C13-1)/(1+(C13-1)*C$3)^2-1),0) &amp; "%"</f>
-        <v>21%</v>
+        <v>24%</v>
       </c>
       <c r="H13" s="2" t="str">
         <f aca="false">ROUND(100*(2^C13/(1+(C13-1)*C$3)^2-1),0) &amp; "%"</f>
-        <v>98%</v>
+        <v>103%</v>
       </c>
       <c r="I13" s="13" t="str">
         <f aca="false">ROUND(100*(1/(1+(C13-1)*C$3)-1),0) &amp; "%"</f>
-        <v>-5%</v>
+        <v>-4%</v>
       </c>
       <c r="J13" s="13" t="str">
         <f aca="false">ROUND(100*((1+(C13-1)*C$3)^(-2)-1),0) &amp; "%"</f>
-        <v>-9%</v>
+        <v>-7%</v>
       </c>
     </row>
     <row r="14" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -563,31 +563,31 @@
       </c>
       <c r="D14" s="12" t="str">
         <f aca="false">ROUND(100*((1+(C14-1)*C$3)^(2/(C14-1))-1),0) &amp; "%"</f>
-        <v>114%</v>
+        <v>78%</v>
       </c>
       <c r="E14" s="2" t="str">
         <f aca="false">ROUND(100*((1+(C14-1)*C$3)^(2/C14)-1),0) &amp; "%"</f>
-        <v>16%</v>
+        <v>12%</v>
       </c>
       <c r="F14" s="2" t="str">
         <f aca="false">ROUND(100*(2^(C14-1)/(1+(C14-1)*C$3)^2-1),0) &amp; "%"</f>
-        <v>-2%</v>
+        <v>3%</v>
       </c>
       <c r="G14" s="2" t="str">
         <f aca="false">ROUND(100*(10^(C14-1)/(1+(C14-1)*C$3)^2-1),0) &amp; "%"</f>
-        <v>47%</v>
+        <v>54%</v>
       </c>
       <c r="H14" s="2" t="str">
         <f aca="false">ROUND(100*(2^C14/(1+(C14-1)*C$3)^2-1),0) &amp; "%"</f>
-        <v>97%</v>
+        <v>106%</v>
       </c>
       <c r="I14" s="13" t="str">
         <f aca="false">ROUND(100*(1/(1+(C14-1)*C$3)-1),0) &amp; "%"</f>
-        <v>-9%</v>
+        <v>-7%</v>
       </c>
       <c r="J14" s="13" t="str">
         <f aca="false">ROUND(100*((1+(C14-1)*C$3)^(-2)-1),0) &amp; "%"</f>
-        <v>-17%</v>
+        <v>-13%</v>
       </c>
     </row>
     <row r="15" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -600,31 +600,31 @@
       </c>
       <c r="D15" s="14" t="str">
         <f aca="false">ROUND(100*((1+(C15-1)*C$3)^(2/(C15-1))-1),0) &amp; "%"</f>
-        <v>107%</v>
+        <v>75%</v>
       </c>
       <c r="E15" s="15" t="str">
         <f aca="false">ROUND(100*((1+(C15-1)*C$3)^(2/C15)-1),0) &amp; "%"</f>
-        <v>28%</v>
+        <v>20%</v>
       </c>
       <c r="F15" s="15" t="str">
         <f aca="false">ROUND(100*(2^(C15-1)/(1+(C15-1)*C$3)^2-1),0) &amp; "%"</f>
-        <v>-2%</v>
+        <v>7%</v>
       </c>
       <c r="G15" s="15" t="str">
         <f aca="false">ROUND(100*(10^(C15-1)/(1+(C15-1)*C$3)^2-1),0) &amp; "%"</f>
-        <v>120%</v>
+        <v>139%</v>
       </c>
       <c r="H15" s="15" t="str">
         <f aca="false">ROUND(100*(2^C15/(1+(C15-1)*C$3)^2-1),0) &amp; "%"</f>
-        <v>96%</v>
+        <v>114%</v>
       </c>
       <c r="I15" s="16" t="str">
         <f aca="false">ROUND(100*(1/(1+(C15-1)*C$3)-1),0) &amp; "%"</f>
-        <v>-17%</v>
+        <v>-13%</v>
       </c>
       <c r="J15" s="16" t="str">
         <f aca="false">ROUND(100*((1+(C15-1)*C$3)^(-2)-1),0) &amp; "%"</f>
-        <v>-31%</v>
+        <v>-24%</v>
       </c>
     </row>
     <row r="16" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -637,31 +637,31 @@
       </c>
       <c r="D16" s="12" t="str">
         <f aca="false">ROUND(100*((1+(C16-1)*C$3)^(2/(C16-1))-1),0) &amp; "%"</f>
-        <v>96%</v>
+        <v>69%</v>
       </c>
       <c r="E16" s="2" t="str">
         <f aca="false">ROUND(100*((1+(C16-1)*C$3)^(2/C16)-1),0) &amp; "%"</f>
-        <v>40%</v>
+        <v>30%</v>
       </c>
       <c r="F16" s="2" t="str">
         <f aca="false">ROUND(100*(2^(C16-1)/(1+(C16-1)*C$3)^2-1),0) &amp; "%"</f>
-        <v>2%</v>
+        <v>18%</v>
       </c>
       <c r="G16" s="2" t="str">
         <f aca="false">ROUND(100*(10^(C16-1)/(1+(C16-1)*C$3)^2-1),0) &amp; "%"</f>
-        <v>410%</v>
+        <v>492%</v>
       </c>
       <c r="H16" s="2" t="str">
         <f aca="false">ROUND(100*(2^C16/(1+(C16-1)*C$3)^2-1),0) &amp; "%"</f>
-        <v>104%</v>
+        <v>137%</v>
       </c>
       <c r="I16" s="13" t="str">
         <f aca="false">ROUND(100*(1/(1+(C16-1)*C$3)-1),0) &amp; "%"</f>
-        <v>-29%</v>
+        <v>-23%</v>
       </c>
       <c r="J16" s="13" t="str">
         <f aca="false">ROUND(100*((1+(C16-1)*C$3)^(-2)-1),0) &amp; "%"</f>
-        <v>-49%</v>
+        <v>-41%</v>
       </c>
     </row>
     <row r="17" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -674,31 +674,31 @@
       </c>
       <c r="D17" s="12" t="str">
         <f aca="false">ROUND(100*((1+(C17-1)*C$3)^(2/(C17-1))-1),0) &amp; "%"</f>
-        <v>80%</v>
+        <v>60%</v>
       </c>
       <c r="E17" s="2" t="str">
         <f aca="false">ROUND(100*((1+(C17-1)*C$3)^(2/C17)-1),0) &amp; "%"</f>
-        <v>48%</v>
+        <v>37%</v>
       </c>
       <c r="F17" s="2" t="str">
         <f aca="false">ROUND(100*(2^(C17-1)/(1+(C17-1)*C$3)^2-1),0) &amp; "%"</f>
-        <v>23%</v>
+        <v>56%</v>
       </c>
       <c r="G17" s="2" t="str">
         <f aca="false">ROUND(100*(10^(C17-1)/(1+(C17-1)*C$3)^2-1),0) &amp; "%"</f>
-        <v>2986%</v>
+        <v>3806%</v>
       </c>
       <c r="H17" s="2" t="str">
         <f aca="false">ROUND(100*(2^C17/(1+(C17-1)*C$3)^2-1),0) &amp; "%"</f>
-        <v>147%</v>
+        <v>212%</v>
       </c>
       <c r="I17" s="13" t="str">
         <f aca="false">ROUND(100*(1/(1+(C17-1)*C$3)-1),0) &amp; "%"</f>
-        <v>-44%</v>
+        <v>-38%</v>
       </c>
       <c r="J17" s="13" t="str">
         <f aca="false">ROUND(100*((1+(C17-1)*C$3)^(-2)-1),0) &amp; "%"</f>
-        <v>-69%</v>
+        <v>-61%</v>
       </c>
     </row>
     <row r="18" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -711,31 +711,31 @@
       </c>
       <c r="D18" s="12" t="str">
         <f aca="false">ROUND(100*((1+(C18-1)*C$3)^(2/(C18-1))-1),0) &amp; "%"</f>
-        <v>61%</v>
+        <v>48%</v>
       </c>
       <c r="E18" s="2" t="str">
         <f aca="false">ROUND(100*((1+(C18-1)*C$3)^(2/C18)-1),0) &amp; "%"</f>
-        <v>47%</v>
+        <v>37%</v>
       </c>
       <c r="F18" s="2" t="str">
         <f aca="false">ROUND(100*(2^(C18-1)/(1+(C18-1)*C$3)^2-1),0) &amp; "%"</f>
-        <v>137%</v>
+        <v>231%</v>
       </c>
       <c r="G18" s="2" t="str">
         <f aca="false">ROUND(100*(10^(C18-1)/(1+(C18-1)*C$3)^2-1),0) &amp; "%"</f>
-        <v>147829%</v>
+        <v>206512%</v>
       </c>
       <c r="H18" s="2" t="str">
         <f aca="false">ROUND(100*(2^C18/(1+(C18-1)*C$3)^2-1),0) &amp; "%"</f>
-        <v>373%</v>
+        <v>561%</v>
       </c>
       <c r="I18" s="13" t="str">
         <f aca="false">ROUND(100*(1/(1+(C18-1)*C$3)-1),0) &amp; "%"</f>
-        <v>-62%</v>
+        <v>-55%</v>
       </c>
       <c r="J18" s="13" t="str">
         <f aca="false">ROUND(100*((1+(C18-1)*C$3)^(-2)-1),0) &amp; "%"</f>
-        <v>-85%</v>
+        <v>-79%</v>
       </c>
     </row>
   </sheetData>

</xml_diff>